<commit_message>
Update U1a and HO1a, add partnership alignment
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C55D118-45C5-4278-B5B4-5D567E3F435B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF5F9C8-8819-4C66-9B08-47CCAA95BE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="8820" yWindow="1905" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -177,10 +177,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,11 +218,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1047,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1062,246 +1067,119 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1994</v>
+      <c r="A2">
+        <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.6613654059472992</v>
+        <v>0.57630000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1995</v>
+      <c r="A3">
+        <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.65666662435166534</v>
+        <v>0.56940000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1996</v>
+      <c r="A4">
+        <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.65162882226991414</v>
+        <v>0.5716</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>1997</v>
+      <c r="A5">
+        <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.64942413470967808</v>
+        <v>0.56459999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1998</v>
+      <c r="A6">
+        <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.64547705146902756</v>
+        <v>0.55630000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>1999</v>
+      <c r="A7">
+        <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.64460168570888343</v>
+        <v>0.54600000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>2000</v>
+      <c r="A8">
+        <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.64477324955863657</v>
+        <v>0.54810000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>2001</v>
+      <c r="A9">
+        <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.64570195231543648</v>
+        <v>0.54100000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>2002</v>
+      <c r="A10">
+        <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.64737782355652385</v>
+        <v>0.55130000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>2003</v>
+      <c r="A11">
+        <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.64448143654604106</v>
+        <v>0.55389999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>2004</v>
+      <c r="A12">
+        <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.64389807700679014</v>
+        <v>0.55249999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>2005</v>
+      <c r="A13">
+        <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.63601678163112885</v>
+        <v>0.55259999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>2006</v>
+      <c r="A14">
+        <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.63885715724636716</v>
+        <v>0.55269999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>2007</v>
+      <c r="A15">
+        <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.63970331929393809</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>2008</v>
-      </c>
-      <c r="B16">
-        <v>0.63745385907812036</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>2009</v>
-      </c>
-      <c r="B17">
-        <v>0.64638142900294271</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>2010</v>
-      </c>
-      <c r="B18">
-        <v>0.64291910814000863</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>2011</v>
-      </c>
-      <c r="B19">
-        <v>0.64183543445918845</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>2012</v>
-      </c>
-      <c r="B20">
-        <v>0.64457311813040019</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>2013</v>
-      </c>
-      <c r="B21">
-        <v>0.64501821298769013</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>2014</v>
-      </c>
-      <c r="B22">
-        <v>0.64303300577959377</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B23">
-        <v>0.64350137796521267</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B24">
-        <v>0.64443090532156433</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>2017</v>
-      </c>
-      <c r="B25">
-        <v>0.64369538754708922</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>2018</v>
-      </c>
-      <c r="B26">
-        <v>0.64389678969687036</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>2019</v>
-      </c>
-      <c r="B27">
-        <v>0.63975244582712099</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>2020</v>
-      </c>
-      <c r="B28">
-        <v>0.64948824720523413</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>2021</v>
-      </c>
-      <c r="B29">
-        <v>0.64443733677754689</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2022</v>
-      </c>
-      <c r="B30">
-        <v>0.64425404141077236</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2023</v>
-      </c>
-      <c r="B31">
-        <v>0.64425404141077236</v>
+        <v>0.55279999999999996</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1809,16 +1687,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Y4" sqref="Y4:Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="23" max="26" width="9.140625" style="3"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -1896,10 +1771,10 @@
       <c r="U3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="X3" t="s">
         <v>40</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1970,13 +1845,13 @@
         <f t="shared" si="0"/>
         <v>23250</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4">
         <v>1994</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4">
         <v>0.49405969999999999</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4">
         <f>2*X4/(2*X4+(1-X4))</f>
         <v>0.6613654059472992</v>
       </c>
@@ -2048,14 +1923,14 @@
         <f t="shared" ref="U5:U12" si="9">I5*$K$4/$K5</f>
         <v>23088.381330685203</v>
       </c>
-      <c r="W5" s="3">
+      <c r="W5">
         <f>W4+1</f>
         <v>1995</v>
       </c>
-      <c r="X5" s="3">
+      <c r="X5">
         <v>0.48883369999999998</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Y5">
         <f t="shared" ref="Y5:Y31" si="10">2*X5/(2*X5+(1-X5))</f>
         <v>0.65666662435166534</v>
       </c>
@@ -2127,14 +2002,14 @@
         <f t="shared" si="9"/>
         <v>22485.493230174081</v>
       </c>
-      <c r="W6" s="3">
-        <f t="shared" ref="W6:W42" si="11">W5+1</f>
+      <c r="W6">
+        <f t="shared" ref="W6:W31" si="11">W5+1</f>
         <v>1996</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6">
         <v>0.48327110000000001</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6">
         <f t="shared" si="10"/>
         <v>0.65162882226991414</v>
       </c>
@@ -2206,14 +2081,14 @@
         <f t="shared" si="9"/>
         <v>21954.67422096317</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7">
         <f t="shared" si="11"/>
         <v>1997</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7">
         <v>0.48084979999999999</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Y7">
         <f t="shared" si="10"/>
         <v>0.64942413470967808</v>
       </c>
@@ -2285,14 +2160,14 @@
         <f t="shared" si="9"/>
         <v>21567.717996289426</v>
       </c>
-      <c r="W8" s="3">
+      <c r="W8">
         <f t="shared" si="11"/>
         <v>1998</v>
       </c>
-      <c r="X8" s="3">
+      <c r="X8">
         <v>0.47653459999999997</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8">
         <f t="shared" si="10"/>
         <v>0.64547705146902756</v>
       </c>
@@ -2364,14 +2239,14 @@
         <f t="shared" si="9"/>
         <v>21389.144434222631</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9">
         <f t="shared" si="11"/>
         <v>1999</v>
       </c>
-      <c r="X9" s="3">
+      <c r="X9">
         <v>0.47558099999999998</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9">
         <f t="shared" si="10"/>
         <v>0.64460168570888343</v>
       </c>
@@ -2443,14 +2318,14 @@
         <f t="shared" si="9"/>
         <v>20833.333333333336</v>
       </c>
-      <c r="W10" s="3">
+      <c r="W10">
         <f t="shared" si="11"/>
         <v>2000</v>
       </c>
-      <c r="X10" s="3">
+      <c r="X10">
         <v>0.47576780000000002</v>
       </c>
-      <c r="Y10" s="3">
+      <c r="Y10">
         <f t="shared" si="10"/>
         <v>0.64477324955863657</v>
       </c>
@@ -2522,14 +2397,14 @@
         <f t="shared" si="9"/>
         <v>19104.354971240755</v>
       </c>
-      <c r="W11" s="3">
+      <c r="W11">
         <f t="shared" si="11"/>
         <v>2001</v>
       </c>
-      <c r="X11" s="3">
+      <c r="X11">
         <v>0.47677979999999998</v>
       </c>
-      <c r="Y11" s="3">
+      <c r="Y11">
         <f t="shared" si="10"/>
         <v>0.64570195231543648</v>
       </c>
@@ -2601,14 +2476,14 @@
         <f t="shared" si="9"/>
         <v>18663.611748853393</v>
       </c>
-      <c r="W12" s="3">
+      <c r="W12">
         <f t="shared" si="11"/>
         <v>2002</v>
       </c>
-      <c r="X12" s="3">
+      <c r="X12">
         <v>0.47860950000000002</v>
       </c>
-      <c r="Y12" s="3">
+      <c r="Y12">
         <f t="shared" si="10"/>
         <v>0.64737782355652385</v>
       </c>
@@ -2662,14 +2537,14 @@
         <f t="shared" ref="U13:U16" si="14">I13*$K$4/$K13</f>
         <v>18360.484915871581</v>
       </c>
-      <c r="W13" s="3">
+      <c r="W13">
         <f t="shared" si="11"/>
         <v>2003</v>
       </c>
-      <c r="X13" s="3">
+      <c r="X13">
         <v>0.47545009999999999</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="Y13">
         <f t="shared" si="10"/>
         <v>0.64448143654604106</v>
       </c>
@@ -2723,14 +2598,14 @@
         <f t="shared" si="14"/>
         <v>18006.917277302477</v>
       </c>
-      <c r="W14" s="3">
+      <c r="W14">
         <f t="shared" si="11"/>
         <v>2004</v>
       </c>
-      <c r="X14" s="3">
+      <c r="X14">
         <v>0.4748154</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="Y14">
         <f t="shared" si="10"/>
         <v>0.64389807700679014</v>
       </c>
@@ -2784,14 +2659,14 @@
         <f t="shared" si="14"/>
         <v>17653.840467943606</v>
       </c>
-      <c r="W15" s="3">
+      <c r="W15">
         <f t="shared" si="11"/>
         <v>2005</v>
       </c>
-      <c r="X15" s="3">
+      <c r="X15">
         <v>0.46629369999999998</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Y15">
         <f t="shared" si="10"/>
         <v>0.63601678163112885</v>
       </c>
@@ -2845,227 +2720,227 @@
         <f t="shared" si="14"/>
         <v>17205.948416783383</v>
       </c>
-      <c r="W16" s="3">
+      <c r="W16">
         <f t="shared" si="11"/>
         <v>2006</v>
       </c>
-      <c r="X16" s="3">
+      <c r="X16">
         <v>0.46935349999999998</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y16">
         <f t="shared" si="10"/>
         <v>0.63885715724636716</v>
       </c>
     </row>
     <row r="17" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W17" s="3">
+      <c r="W17">
         <f t="shared" si="11"/>
         <v>2007</v>
       </c>
-      <c r="X17" s="3">
+      <c r="X17">
         <v>0.4702675</v>
       </c>
-      <c r="Y17" s="3">
+      <c r="Y17">
         <f t="shared" si="10"/>
         <v>0.63970331929393809</v>
       </c>
     </row>
     <row r="18" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W18" s="3">
+      <c r="W18">
         <f t="shared" si="11"/>
         <v>2008</v>
       </c>
-      <c r="X18" s="3">
+      <c r="X18">
         <v>0.46784019999999998</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="Y18">
         <f t="shared" si="10"/>
         <v>0.63745385907812036</v>
       </c>
     </row>
     <row r="19" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W19" s="3">
+      <c r="W19">
         <f t="shared" si="11"/>
         <v>2009</v>
       </c>
-      <c r="X19" s="3">
+      <c r="X19">
         <v>0.47752109999999998</v>
       </c>
-      <c r="Y19" s="3">
+      <c r="Y19">
         <f t="shared" si="10"/>
         <v>0.64638142900294271</v>
       </c>
     </row>
     <row r="20" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W20" s="3">
+      <c r="W20">
         <f t="shared" si="11"/>
         <v>2010</v>
       </c>
-      <c r="X20" s="3">
+      <c r="X20">
         <v>0.47375149999999999</v>
       </c>
-      <c r="Y20" s="3">
+      <c r="Y20">
         <f t="shared" si="10"/>
         <v>0.64291910814000863</v>
       </c>
     </row>
     <row r="21" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W21" s="3">
+      <c r="W21">
         <f t="shared" si="11"/>
         <v>2011</v>
       </c>
-      <c r="X21" s="3">
+      <c r="X21">
         <v>0.47257559999999998</v>
       </c>
-      <c r="Y21" s="3">
+      <c r="Y21">
         <f t="shared" si="10"/>
         <v>0.64183543445918845</v>
       </c>
     </row>
     <row r="22" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W22" s="3">
+      <c r="W22">
         <f t="shared" si="11"/>
         <v>2012</v>
       </c>
-      <c r="X22" s="3">
+      <c r="X22">
         <v>0.47554990000000003</v>
       </c>
-      <c r="Y22" s="3">
+      <c r="Y22">
         <f t="shared" si="10"/>
         <v>0.64457311813040019</v>
       </c>
     </row>
     <row r="23" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W23" s="3">
+      <c r="W23">
         <f t="shared" si="11"/>
         <v>2013</v>
       </c>
-      <c r="X23" s="3">
+      <c r="X23">
         <v>0.47603459999999997</v>
       </c>
-      <c r="Y23" s="3">
+      <c r="Y23">
         <f t="shared" si="10"/>
         <v>0.64501821298769013</v>
       </c>
     </row>
     <row r="24" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W24" s="3">
+      <c r="W24">
         <f t="shared" si="11"/>
         <v>2014</v>
       </c>
-      <c r="X24" s="3">
+      <c r="X24">
         <v>0.4738752</v>
       </c>
-      <c r="Y24" s="3">
+      <c r="Y24">
         <f t="shared" si="10"/>
         <v>0.64303300577959377</v>
       </c>
     </row>
     <row r="25" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W25" s="3">
+      <c r="W25">
         <f t="shared" si="11"/>
         <v>2015</v>
       </c>
-      <c r="X25" s="3">
+      <c r="X25">
         <v>0.47438409999999998</v>
       </c>
-      <c r="Y25" s="3">
+      <c r="Y25">
         <f t="shared" si="10"/>
         <v>0.64350137796521267</v>
       </c>
     </row>
     <row r="26" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W26" s="3">
+      <c r="W26">
         <f t="shared" si="11"/>
         <v>2016</v>
       </c>
-      <c r="X26" s="3">
+      <c r="X26">
         <v>0.47539510000000001</v>
       </c>
-      <c r="Y26" s="3">
+      <c r="Y26">
         <f t="shared" si="10"/>
         <v>0.64443090532156433</v>
       </c>
     </row>
     <row r="27" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W27" s="3">
+      <c r="W27">
         <f t="shared" si="11"/>
         <v>2017</v>
       </c>
-      <c r="X27" s="3">
+      <c r="X27">
         <v>0.47459499999999999</v>
       </c>
-      <c r="Y27" s="3">
+      <c r="Y27">
         <f t="shared" si="10"/>
         <v>0.64369538754708922</v>
       </c>
     </row>
     <row r="28" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W28" s="3">
+      <c r="W28">
         <f t="shared" si="11"/>
         <v>2018</v>
       </c>
-      <c r="X28" s="3">
+      <c r="X28">
         <v>0.47481400000000001</v>
       </c>
-      <c r="Y28" s="3">
+      <c r="Y28">
         <f t="shared" si="10"/>
         <v>0.64389678969687036</v>
       </c>
     </row>
     <row r="29" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W29" s="3">
+      <c r="W29">
         <f t="shared" si="11"/>
         <v>2019</v>
       </c>
-      <c r="X29" s="3">
+      <c r="X29">
         <v>0.47032059999999998</v>
       </c>
-      <c r="Y29" s="3">
+      <c r="Y29">
         <f t="shared" si="10"/>
         <v>0.63975244582712099</v>
       </c>
     </row>
     <row r="30" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W30" s="3">
+      <c r="W30">
         <f t="shared" si="11"/>
         <v>2020</v>
       </c>
-      <c r="X30" s="3">
+      <c r="X30">
         <v>0.48092010000000002</v>
       </c>
-      <c r="Y30" s="3">
+      <c r="Y30">
         <f t="shared" si="10"/>
         <v>0.64948824720523413</v>
       </c>
     </row>
     <row r="31" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W31" s="3">
+      <c r="W31">
         <f t="shared" si="11"/>
         <v>2021</v>
       </c>
-      <c r="X31" s="3">
+      <c r="X31">
         <v>0.47540209999999999</v>
       </c>
-      <c r="Y31" s="3">
+      <c r="Y31">
         <f t="shared" si="10"/>
         <v>0.64443733677754689</v>
       </c>
     </row>
     <row r="32" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W32" s="3">
+      <c r="W32">
         <v>2022</v>
       </c>
-      <c r="Y32" s="3">
+      <c r="Y32">
         <f>AVERAGE(Y27:Y31)</f>
         <v>0.64425404141077236</v>
       </c>
     </row>
     <row r="33" spans="23:25" x14ac:dyDescent="0.25">
-      <c r="W33" s="3">
+      <c r="W33">
         <v>2023</v>
       </c>
-      <c r="Y33" s="3">
+      <c r="Y33">
         <f>Y32</f>
         <v>0.64425404141077236</v>
       </c>

</xml_diff>

<commit_message>
Introduce alignment of retirement status. Correct liwwh.
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E2C769-986C-4A6B-90C6-6DB425FE6931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427F635B-1DDB-4481-817B-442FECC2148B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="social care" sheetId="1" r:id="rId2"/>
-    <sheet name="partnership" sheetId="4" r:id="rId3"/>
-    <sheet name="employment_smales" sheetId="5" r:id="rId4"/>
-    <sheet name="employment_sfemales" sheetId="6" r:id="rId5"/>
-    <sheet name="employment_couples" sheetId="7" r:id="rId6"/>
-    <sheet name="raw data" sheetId="3" r:id="rId7"/>
+    <sheet name="retirement" sheetId="8" r:id="rId3"/>
+    <sheet name="partnership" sheetId="4" r:id="rId4"/>
+    <sheet name="employment_smales" sheetId="5" r:id="rId5"/>
+    <sheet name="employment_sfemales" sheetId="6" r:id="rId6"/>
+    <sheet name="employment_couples" sheetId="7" r:id="rId7"/>
+    <sheet name="raw data" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -1054,7 +1055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542CF42B-7BCB-429C-A72F-92D7D9CDCB1D}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1074,6 +1075,139 @@
         <v>2010</v>
       </c>
       <c r="B2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.20599999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
         <v>0.60599999999999998</v>
       </c>
     </row>
@@ -1187,7 +1321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -1354,7 +1488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -1521,7 +1655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -1688,7 +1822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
   <dimension ref="A1:Y33"/>
   <sheetViews>

</xml_diff>

<commit_message>
Introduce student status alignment method
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427F635B-1DDB-4481-817B-442FECC2148B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0556C1A0-0DFC-4874-BC77-7169EA7F0634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="8580" yWindow="4035" windowWidth="28800" windowHeight="15105" activeTab="3" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="social care" sheetId="1" r:id="rId2"/>
     <sheet name="retirement" sheetId="8" r:id="rId3"/>
-    <sheet name="partnership" sheetId="4" r:id="rId4"/>
-    <sheet name="employment_smales" sheetId="5" r:id="rId5"/>
-    <sheet name="employment_sfemales" sheetId="6" r:id="rId6"/>
-    <sheet name="employment_couples" sheetId="7" r:id="rId7"/>
-    <sheet name="raw data" sheetId="3" r:id="rId8"/>
+    <sheet name="students" sheetId="9" r:id="rId4"/>
+    <sheet name="partnership" sheetId="4" r:id="rId5"/>
+    <sheet name="employment_smales" sheetId="5" r:id="rId6"/>
+    <sheet name="employment_sfemales" sheetId="6" r:id="rId7"/>
+    <sheet name="employment_couples" sheetId="7" r:id="rId8"/>
+    <sheet name="raw data" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -1058,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542CF42B-7BCB-429C-A72F-92D7D9CDCB1D}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1188,6 +1189,141 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D18F52-AE20-431C-A8C1-CEFDA270A8FD}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.19700000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1321,7 +1457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -1488,7 +1624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -1655,7 +1791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -1822,7 +1958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
   <dimension ref="A1:Y33"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update employment alignment targets
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F6CE4-63F4-4F2E-B8F7-A33A358ECED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2BE7F8-84EB-4E32-A6F1-96A5F0E23BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="5" activeTab="8" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="disability" sheetId="10" r:id="rId1"/>
@@ -544,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BE8D09-68C3-47E4-AB1B-09AAE2124BA2}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2863,7 +2863,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B19"/>
+      <selection activeCell="B14" sqref="B14:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2881,7 +2881,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.53940549999999998</v>
+        <v>0.63684130000000005</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2889,7 +2889,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.54004809999999992</v>
+        <v>0.63684130000000005</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2897,7 +2897,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.55193539999999996</v>
+        <v>0.63086129999999996</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.57619909999999996</v>
+        <v>0.62820810000000005</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.57942509999999992</v>
+        <v>0.63444250000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2921,7 +2921,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.57820819999999995</v>
+        <v>0.64983950000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.57820819999999995</v>
+        <v>0.66639119999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2937,7 +2937,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.57820819999999995</v>
+        <v>0.67221770000000003</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.57820819999999995</v>
+        <v>0.67153039999999997</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2953,7 +2953,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.57820819999999995</v>
+        <v>0.67241660000000003</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2961,7 +2961,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.57820819999999995</v>
+        <v>0.69137210000000004</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2969,7 +2969,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.57820819999999995</v>
+        <v>0.703434</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.57820819999999995</v>
+        <v>0.69511619999999996</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2985,7 +2985,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.57820819999999995</v>
+        <v>0.69436249999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.57820819999999995</v>
+        <v>0.69360880000000003</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3001,7 +3001,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.57820819999999995</v>
+        <v>0.69285509999999995</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3009,7 +3009,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.57820819999999995</v>
+        <v>0.69210139999999998</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3017,7 +3017,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.57820819999999995</v>
+        <v>0.69134770000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3030,7 +3030,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B14" sqref="B14:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3048,7 +3048,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.39165939999999999</v>
+        <v>0.39854529999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.40846290000000002</v>
+        <v>0.39854529999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.41123969999999999</v>
+        <v>0.4029663</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.43660460000000001</v>
+        <v>0.39655180000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.44596649999999999</v>
+        <v>0.4070319</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.45383590000000001</v>
+        <v>0.40790100000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.45383590000000001</v>
+        <v>0.41726039999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3104,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.45383590000000001</v>
+        <v>0.42810779999999998</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.45383590000000001</v>
+        <v>0.42215740000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.45383590000000001</v>
+        <v>0.41901169999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.45383590000000001</v>
+        <v>0.42423159999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.45383590000000001</v>
+        <v>0.41884729999999998</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.45383590000000001</v>
+        <v>0.42949969999999998</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,7 +3152,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.45383590000000001</v>
+        <v>0.42430040000000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,7 +3160,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.45383590000000001</v>
+        <v>0.4191011</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.45383590000000001</v>
+        <v>0.41390179999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.45383590000000001</v>
+        <v>0.40870250000000002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.45383590000000001</v>
+        <v>0.40350320000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3196,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3215,7 +3215,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.71755429999999998</v>
+        <v>0.7511234</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3223,7 +3223,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.73036599999999996</v>
+        <v>0.7511234</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3231,7 +3231,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.74233179999999999</v>
+        <v>0.74668140000000005</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,7 +3239,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.74778829999999996</v>
+        <v>0.74351520000000004</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3247,7 +3247,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.74564959999999991</v>
+        <v>0.74422900000000003</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3255,7 +3255,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.74624679999999999</v>
+        <v>0.73707429999999996</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.74345260000000002</v>
+        <v>0.74269050000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.74345260000000002</v>
+        <v>0.74164249999999998</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.74345260000000002</v>
+        <v>0.73936999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.74345260000000002</v>
+        <v>0.7404522</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3295,7 +3295,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.74345260000000002</v>
+        <v>0.72219089999999997</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3303,7 +3303,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.74345260000000002</v>
+        <v>0.72516029999999998</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3311,7 +3311,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.74345260000000002</v>
+        <v>0.74010039999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.74345260000000002</v>
+        <v>0.73162090000000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.74345260000000002</v>
+        <v>0.738754466666667</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3335,7 +3335,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.74345260000000002</v>
+        <v>0.74198476666666702</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3343,7 +3343,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.74345260000000002</v>
+        <v>0.74521506666666704</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3351,7 +3351,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.74345260000000002</v>
+        <v>0.74844536666666694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to activity alignment
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2BE7F8-84EB-4E32-A6F1-96A5F0E23BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1117CD45-C575-4074-A068-96F2E7D9BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="5" activeTab="8" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="20280" activeTab="4" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="disability" sheetId="10" r:id="rId1"/>
@@ -2591,610 +2591,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D18F52-AE20-431C-A8C1-CEFDA270A8FD}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.23899999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3">
-        <v>0.23899999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
-        <v>0.23400000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>0.22600000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
-        <v>0.219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
-        <v>0.218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
-        <v>0.21299999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
-        <v>0.20499999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>0.20399999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
-        <v>0.19700000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14">
-        <v>0.19500000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.188</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.60599999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3">
-        <v>0.60860000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
-        <v>0.60570000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
-        <v>0.61019999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>0.61339999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
-        <v>0.61570000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
-        <v>0.61919999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
-        <v>0.62190000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
-        <v>0.624</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
-        <v>0.62809999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>0.64049999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
-        <v>0.62729999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14">
-        <v>0.62050000000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.61850000000000005</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
-  <dimension ref="A1:B19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.63684130000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3">
-        <v>0.63684130000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
-        <v>0.63086129999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
-        <v>0.62820810000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>0.63444250000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
-        <v>0.64983950000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
-        <v>0.66639119999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
-        <v>0.67221770000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
-        <v>0.67153039999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
-        <v>0.67241660000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>0.69137210000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
-        <v>0.703434</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14">
-        <v>0.69511619999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.69436249999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2024</v>
-      </c>
-      <c r="B16">
-        <v>0.69360880000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2025</v>
-      </c>
-      <c r="B17">
-        <v>0.69285509999999995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2026</v>
-      </c>
-      <c r="B18">
-        <v>0.69210139999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2027</v>
-      </c>
-      <c r="B19">
-        <v>0.69134770000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
-  <dimension ref="A1:B19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.39854529999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3">
-        <v>0.39854529999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
-        <v>0.4029663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
-        <v>0.39655180000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>0.4070319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
-        <v>0.40790100000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
-        <v>0.41726039999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
-        <v>0.42810779999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
-        <v>0.42215740000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
-        <v>0.41901169999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>0.42423159999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
-        <v>0.41884729999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14">
-        <v>0.42949969999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.42430040000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2024</v>
-      </c>
-      <c r="B16">
-        <v>0.4191011</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2025</v>
-      </c>
-      <c r="B17">
-        <v>0.41390179999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2026</v>
-      </c>
-      <c r="B18">
-        <v>0.40870250000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2027</v>
-      </c>
-      <c r="B19">
-        <v>0.40350320000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -3204,10 +2601,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3215,7 +2612,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.7511234</v>
+        <v>0.23899999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3223,7 +2620,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.7511234</v>
+        <v>0.23899999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3231,7 +2628,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.74668140000000005</v>
+        <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,7 +2636,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.74351520000000004</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3247,7 +2644,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.74422900000000003</v>
+        <v>0.22600000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3255,7 +2652,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.73707429999999996</v>
+        <v>0.219</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,7 +2660,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.74269050000000003</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3271,7 +2668,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.74164249999999998</v>
+        <v>0.21299999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3279,7 +2676,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.73936999999999997</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3287,7 +2684,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.7404522</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3295,7 +2692,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.72219089999999997</v>
+        <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -3303,7 +2700,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.72516029999999998</v>
+        <v>0.19700000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -3311,7 +2708,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.74010039999999999</v>
+        <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3319,7 +2716,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.73162090000000002</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3327,7 +2724,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.738754466666667</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3335,7 +2732,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.74198476666666702</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3343,7 +2740,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.74521506666666704</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3351,7 +2748,996 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.74844536666666694</v>
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2028</v>
+      </c>
+      <c r="B20">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2029</v>
+      </c>
+      <c r="B21">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2031</v>
+      </c>
+      <c r="B23">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2032</v>
+      </c>
+      <c r="B24">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2033</v>
+      </c>
+      <c r="B25">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2034</v>
+      </c>
+      <c r="B26">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2035</v>
+      </c>
+      <c r="B27">
+        <v>0.188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.60860000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.60570000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.61019999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.61339999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.61570000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.61919999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.62190000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.62809999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.64049999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.62729999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.62050000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2028</v>
+      </c>
+      <c r="B20">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2029</v>
+      </c>
+      <c r="B21">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2031</v>
+      </c>
+      <c r="B23">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2032</v>
+      </c>
+      <c r="B24">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2033</v>
+      </c>
+      <c r="B25">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2034</v>
+      </c>
+      <c r="B26">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2035</v>
+      </c>
+      <c r="B27">
+        <v>0.61850000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.63684130000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.63684130000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.63086129999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.62820810000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.63444250000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.64983950000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.66639119999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.67221770000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.67153039999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.67241660000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.69137210000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.703434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.70015435151515204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.70666020046620004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.71316604941724904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.71967189836829804</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.72617774731934703</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.73268359627039603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2028</v>
+      </c>
+      <c r="B20">
+        <v>0.73918944522144503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2029</v>
+      </c>
+      <c r="B21">
+        <v>0.74569529417249403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22">
+        <v>0.75220114312354303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2031</v>
+      </c>
+      <c r="B23">
+        <v>0.75870699207459202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2032</v>
+      </c>
+      <c r="B24">
+        <v>0.76521284102564102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2033</v>
+      </c>
+      <c r="B25">
+        <v>0.77171868997669002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2034</v>
+      </c>
+      <c r="B26">
+        <v>0.77822453892773902</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2035</v>
+      </c>
+      <c r="B27">
+        <v>0.78473038787878802</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.39854529999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.39854529999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.4029663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.39655180000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.4070319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.40790100000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.41726039999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.42810779999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.42215740000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.41901169999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.42423159999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.41884729999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.42949969999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.43197885000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.4346719</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.43736494999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.440058</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.44275104999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2028</v>
+      </c>
+      <c r="B20">
+        <v>0.44544410000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2029</v>
+      </c>
+      <c r="B21">
+        <v>0.44813714999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22">
+        <v>0.45083020000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2031</v>
+      </c>
+      <c r="B23">
+        <v>0.45352324999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2032</v>
+      </c>
+      <c r="B24">
+        <v>0.45621630000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2033</v>
+      </c>
+      <c r="B25">
+        <v>0.45890934999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2034</v>
+      </c>
+      <c r="B26">
+        <v>0.46160240000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2035</v>
+      </c>
+      <c r="B27">
+        <v>0.46429545</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.7511234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.7511234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.74668140000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.74351520000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.74422900000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.73707429999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.74269050000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.74164249999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.73936999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.7404522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.73668559333333306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.73539384848484901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.73410210363636397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.73281035878787903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.73151861393939399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.73022686909090895</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.72893512424242402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.72764337939393897</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2028</v>
+      </c>
+      <c r="B20">
+        <v>0.72635163454545504</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2029</v>
+      </c>
+      <c r="B21">
+        <v>0.72505988969696999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22">
+        <v>0.72376814484848495</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2031</v>
+      </c>
+      <c r="B23">
+        <v>0.72247640000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2032</v>
+      </c>
+      <c r="B24">
+        <v>0.72247640000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2033</v>
+      </c>
+      <c r="B25">
+        <v>0.72247640000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2034</v>
+      </c>
+      <c r="B26">
+        <v>0.72247640000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2035</v>
+      </c>
+      <c r="B27">
+        <v>0.72247640000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>